<commit_message>
Tooltips and fixed dates.
</commit_message>
<xml_diff>
--- a/data/IndexPresets.xlsx
+++ b/data/IndexPresets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian(SatovskyAsset\Desktop\Projects\WealthManagementDashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6344A4C3-7105-454C-A76E-5566BD7DA967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308D84CD-4402-4DAB-B74B-F79D0DA907D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14055" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1374" yWindow="1422" windowWidth="17280" windowHeight="9984" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>label</t>
   </si>
@@ -68,6 +68,42 @@
   </si>
   <si>
     <t>The index's standard deviation in %.</t>
+  </si>
+  <si>
+    <t>SAM 100</t>
+  </si>
+  <si>
+    <t>SAM 85/15</t>
+  </si>
+  <si>
+    <t>SAM 70/30</t>
+  </si>
+  <si>
+    <t>SAM 60/40</t>
+  </si>
+  <si>
+    <t>SAM 45/55</t>
+  </si>
+  <si>
+    <t>SAM 30/70</t>
+  </si>
+  <si>
+    <t>sam100</t>
+  </si>
+  <si>
+    <t>sam8515</t>
+  </si>
+  <si>
+    <t>sam7030</t>
+  </si>
+  <si>
+    <t>sam6040</t>
+  </si>
+  <si>
+    <t>sam4555</t>
+  </si>
+  <si>
+    <t>sam3070</t>
   </si>
 </sst>
 </file>
@@ -111,9 +147,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,7 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A1F3D2-F34D-42E1-83D4-B98D8EC995C4}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -449,16 +488,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="7.3125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.47265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5234375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.9453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.3671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -519,6 +558,90 @@
         <v>15.28</v>
       </c>
     </row>
+    <row r="5" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D5" s="2">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7.94</v>
+      </c>
+      <c r="D6" s="2">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2">
+        <v>7.02</v>
+      </c>
+      <c r="D7" s="2">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2">
+        <v>6.18</v>
+      </c>
+      <c r="D8" s="2">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2">
+        <v>5.26</v>
+      </c>
+      <c r="D9" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4.13</v>
+      </c>
+      <c r="D10" s="2">
+        <v>4.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added covariance for some assets
</commit_message>
<xml_diff>
--- a/data/IndexPresets.xlsx
+++ b/data/IndexPresets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian(SatovskyAsset\Desktop\Projects\WealthManagementDashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308D84CD-4402-4DAB-B74B-F79D0DA907D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BDD624-4179-4F91-A6D6-0D5DA45149CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1374" yWindow="1422" windowWidth="17280" windowHeight="9984" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="366" yWindow="366" windowWidth="17280" windowHeight="9984" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>label</t>
   </si>
@@ -40,22 +40,10 @@
     <t>standard deviation</t>
   </si>
   <si>
-    <t>VTI</t>
-  </si>
-  <si>
-    <t>vti</t>
-  </si>
-  <si>
-    <t>ITOT</t>
-  </si>
-  <si>
     <t>S&amp;P 500</t>
   </si>
   <si>
     <t>sp500</t>
-  </si>
-  <si>
-    <t>itot</t>
   </si>
   <si>
     <t>The text visible on the dropdown menu.</t>
@@ -448,7 +436,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -458,7 +446,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -468,7 +456,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -478,7 +466,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -488,10 +476,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -524,121 +512,93 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>10.66</v>
+        <v>11.03</v>
       </c>
       <c r="D2">
-        <v>15.56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>12.24</v>
-      </c>
-      <c r="D3">
-        <v>15.62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>11.03</v>
-      </c>
-      <c r="D4">
         <v>15.28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D3" s="2">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2">
+        <v>7.94</v>
+      </c>
+      <c r="D4" s="2">
+        <v>12.9</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2">
-        <v>8.6999999999999993</v>
+        <v>7.02</v>
       </c>
       <c r="D5" s="2">
-        <v>14.8</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2">
-        <v>7.94</v>
+        <v>6.18</v>
       </c>
       <c r="D6" s="2">
-        <v>12.9</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
-        <v>7.02</v>
+        <v>5.26</v>
       </c>
       <c r="D7" s="2">
-        <v>10.8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2">
-        <v>6.18</v>
+        <v>4.13</v>
       </c>
       <c r="D8" s="2">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2">
-        <v>5.26</v>
-      </c>
-      <c r="D9" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2">
-        <v>4.13</v>
-      </c>
-      <c r="D10" s="2">
         <v>4.8</v>
       </c>
     </row>

</xml_diff>